<commit_message>
Fixing Saurin, please send goat.
</commit_message>
<xml_diff>
--- a/data_files/grad_rate.xlsx
+++ b/data_files/grad_rate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saurin/Desktop/Project-1/new_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saurin/Desktop/Project-1/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724EBFBC-B45A-5F4B-A5E2-67EFE78109DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D29F76C-343B-544C-90B0-374111B81E81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16100" xr2:uid="{6CE29CD1-03A5-8E41-8A56-FC33D5F22698}"/>
   </bookViews>
@@ -305,7 +305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -316,22 +316,25 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,10 +650,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928E3AA9-5293-2B4D-B919-85CFE616C078}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -660,36 +664,42 @@
     <col min="8" max="8" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19">
+    <row r="1" spans="1:11" ht="19">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="19">
+    <row r="2" spans="1:11" ht="19">
       <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="10">
         <v>2010</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="10">
         <v>2011</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="10">
         <v>2012</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="10">
         <v>2013</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="10">
         <v>2014</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="11">
         <v>2015</v>
       </c>
-      <c r="H2" s="17">
+      <c r="H2" s="11">
         <v>2016</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="17">
+      <c r="I2" s="10">
+        <v>2017</v>
+      </c>
+      <c r="J2" s="10">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="17">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -715,333 +725,350 @@
         <v>85.4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:11">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="12">
         <v>72</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="12">
         <v>75</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="12">
         <v>80</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="12">
         <v>75</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="13">
         <v>89.3</v>
       </c>
-      <c r="G4" s="12">
-        <v>87</v>
-      </c>
-      <c r="H4">
+      <c r="G4" s="14">
+        <v>87</v>
+      </c>
+      <c r="H4" s="3">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:11">
       <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="12">
         <v>68</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="12">
         <v>70</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="12">
         <v>71.8</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="12">
         <v>70</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="13">
         <v>75.599999999999994</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="14">
         <v>76</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:11">
       <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="12">
         <v>78</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="12">
         <v>76</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="12">
         <v>75.099999999999994</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="12">
         <v>76</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="13">
         <v>77.400000000000006</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="14">
         <v>8</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:11">
       <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="12">
         <v>81</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="12">
         <v>84</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="12">
         <v>84.9</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="12">
         <v>84</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="13">
         <v>84.9</v>
       </c>
-      <c r="G7" s="12">
-        <v>87</v>
-      </c>
-      <c r="H7">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="G7" s="14">
+        <v>87</v>
+      </c>
+      <c r="H7" s="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="12">
         <v>76</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="12">
         <v>79</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="12">
         <v>80.400000000000006</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="12">
         <v>79</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="13">
         <v>82</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="14">
         <v>83</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:11">
       <c r="A9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="12">
         <v>74</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="12">
         <v>75</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="12">
         <v>76.900000000000006</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="12">
         <v>75</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="13">
         <v>77.3</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="14">
         <v>79</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:11">
       <c r="A10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="12">
         <v>83</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="12">
         <v>85</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="12">
         <v>85.5</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="12">
         <v>85</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="13">
         <v>87.2</v>
       </c>
-      <c r="G10" s="12">
-        <v>87</v>
-      </c>
-      <c r="H10">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="G10" s="14">
+        <v>87</v>
+      </c>
+      <c r="H10" s="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="12">
         <v>78</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="12">
         <v>80</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="12">
         <v>80.400000000000006</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="12">
         <v>80</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="13">
         <v>85.6</v>
       </c>
-      <c r="G11" s="12">
-        <v>86</v>
-      </c>
-      <c r="H11">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="G11" s="14">
+        <v>86</v>
+      </c>
+      <c r="H11" s="3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="12">
         <v>59</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="12">
         <v>59</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="12">
         <v>62.3</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="12">
         <v>59</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="13">
         <v>68.5</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="14">
         <v>69</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="3">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:11">
       <c r="A13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="12">
         <v>71</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="12">
         <v>75</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="12">
         <v>75.599999999999994</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="12">
         <v>75</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="13">
         <v>77.900000000000006</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="14">
         <v>81</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:11">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="12">
         <v>67</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="12">
         <v>70</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="12">
         <v>71.7</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="12">
         <v>70</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="13">
         <v>78.8</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="14">
         <v>79</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>81</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" s="18">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="J14" s="18">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="K14" s="18">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="12">
         <v>80</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="12">
         <v>81</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="12">
         <v>82.4</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="12">
         <v>81</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="13">
         <v>81.599999999999994</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="14">
         <v>83</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:11">
       <c r="A16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="11">
+      <c r="B16" s="15">
+        <v>79.63</v>
+      </c>
+      <c r="C16" s="15">
+        <v>79.63</v>
+      </c>
+      <c r="D16" s="15">
+        <v>79.63</v>
+      </c>
+      <c r="E16" s="15">
+        <v>79.63</v>
+      </c>
+      <c r="F16" s="13">
         <v>78.900000000000006</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="14">
         <v>80</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="3">
         <v>80</v>
       </c>
     </row>
@@ -1049,25 +1076,25 @@
       <c r="A17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="12">
         <v>84</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="12">
         <v>82</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="12">
         <v>83.2</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="12">
         <v>82</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="13">
         <v>85.6</v>
       </c>
-      <c r="G17" s="12">
-        <v>86</v>
-      </c>
-      <c r="H17">
+      <c r="G17" s="14">
+        <v>86</v>
+      </c>
+      <c r="H17" s="3">
         <v>87</v>
       </c>
     </row>
@@ -1075,25 +1102,25 @@
       <c r="A18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="10">
-        <v>86</v>
-      </c>
-      <c r="C18" s="10">
-        <v>86</v>
-      </c>
-      <c r="D18" s="10">
-        <v>87</v>
-      </c>
-      <c r="E18" s="10">
-        <v>86</v>
-      </c>
-      <c r="F18" s="11">
+      <c r="B18" s="12">
+        <v>86</v>
+      </c>
+      <c r="C18" s="12">
+        <v>86</v>
+      </c>
+      <c r="D18" s="12">
+        <v>87</v>
+      </c>
+      <c r="E18" s="12">
+        <v>86</v>
+      </c>
+      <c r="F18" s="13">
         <v>87.1</v>
       </c>
-      <c r="G18" s="12">
-        <v>87</v>
-      </c>
-      <c r="H18">
+      <c r="G18" s="14">
+        <v>87</v>
+      </c>
+      <c r="H18" s="3">
         <v>84</v>
       </c>
     </row>
@@ -1101,25 +1128,25 @@
       <c r="A19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="10">
-        <v>88</v>
-      </c>
-      <c r="C19" s="10">
+      <c r="B19" s="12">
+        <v>88</v>
+      </c>
+      <c r="C19" s="12">
         <v>89</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="12">
         <v>89.7</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="12">
         <v>89</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="13">
         <v>90.8</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="14">
         <v>91</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="3">
         <v>91</v>
       </c>
     </row>
@@ -1127,25 +1154,25 @@
       <c r="A20" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="12">
         <v>83</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="12">
         <v>85</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="12">
         <v>85.7</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="12">
         <v>85</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="13">
         <v>85.7</v>
       </c>
-      <c r="G20" s="12">
-        <v>86</v>
-      </c>
-      <c r="H20">
+      <c r="G20" s="14">
+        <v>86</v>
+      </c>
+      <c r="H20" s="3">
         <v>87</v>
       </c>
     </row>
@@ -1153,19 +1180,25 @@
       <c r="A21" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="10">
+      <c r="B21" s="12">
+        <v>88.27</v>
+      </c>
+      <c r="C21" s="12">
+        <v>88.27</v>
+      </c>
+      <c r="D21" s="12">
         <v>86.1</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="11">
-        <v>88</v>
-      </c>
-      <c r="G21" s="12">
+      <c r="E21" s="15">
+        <v>88.27</v>
+      </c>
+      <c r="F21" s="13">
+        <v>88</v>
+      </c>
+      <c r="G21" s="14">
         <v>89</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="3">
         <v>90</v>
       </c>
     </row>
@@ -1173,25 +1206,25 @@
       <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="12">
         <v>71</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="12">
         <v>72</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="12">
         <v>73.5</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="12">
         <v>72</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="13">
         <v>77.5</v>
       </c>
-      <c r="G22" s="12">
+      <c r="G22" s="14">
         <v>79</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="3">
         <v>78</v>
       </c>
     </row>
@@ -1199,25 +1232,25 @@
       <c r="A23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="12">
         <v>84</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="12">
         <v>85</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="12">
         <v>86.4</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="12">
         <v>85</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="13">
         <v>87.5</v>
       </c>
-      <c r="G23" s="12">
-        <v>87</v>
-      </c>
-      <c r="H23">
+      <c r="G23" s="14">
+        <v>87</v>
+      </c>
+      <c r="H23" s="3">
         <v>87</v>
       </c>
     </row>
@@ -1225,25 +1258,25 @@
       <c r="A24" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="12">
         <v>83</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="12">
         <v>84</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="12">
         <v>85</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="12">
         <v>84</v>
       </c>
-      <c r="F24" s="11">
-        <v>87</v>
-      </c>
-      <c r="G24" s="12">
-        <v>88</v>
-      </c>
-      <c r="H24">
+      <c r="F24" s="13">
+        <v>87</v>
+      </c>
+      <c r="G24" s="14">
+        <v>88</v>
+      </c>
+      <c r="H24" s="3">
         <v>88</v>
       </c>
     </row>
@@ -1251,25 +1284,25 @@
       <c r="A25" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="12">
         <v>83</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="12">
         <v>85</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="12">
         <v>85</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="12">
         <v>85</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="13">
         <v>87.3</v>
       </c>
-      <c r="G25" s="12">
-        <v>88</v>
-      </c>
-      <c r="H25">
+      <c r="G25" s="14">
+        <v>88</v>
+      </c>
+      <c r="H25" s="3">
         <v>88</v>
       </c>
     </row>
@@ -1277,25 +1310,25 @@
       <c r="A26" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="12">
         <v>74</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="12">
         <v>76</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="12">
         <v>77</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="12">
         <v>76</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="13">
         <v>79.8</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="14">
         <v>80</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="3">
         <v>80</v>
       </c>
     </row>
@@ -1303,25 +1336,25 @@
       <c r="A27" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="12">
         <v>77</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="12">
         <v>78</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="12">
         <v>79.8</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="12">
         <v>78</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="13">
         <v>81.900000000000006</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G27" s="14">
         <v>82</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="3">
         <v>83</v>
       </c>
     </row>
@@ -1329,25 +1362,25 @@
       <c r="A28" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="12">
         <v>75</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="12">
         <v>75</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="12">
         <v>75.5</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="12">
         <v>75</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="13">
         <v>80.800000000000011</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="14">
         <v>82</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="3">
         <v>83</v>
       </c>
     </row>
@@ -1355,25 +1388,25 @@
       <c r="A29" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="12">
         <v>81</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="12">
         <v>84</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="12">
         <v>85.7</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="12">
         <v>84</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="13">
         <v>87.8</v>
       </c>
-      <c r="G29" s="12">
+      <c r="G29" s="14">
         <v>89</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="3">
         <v>88</v>
       </c>
     </row>
@@ -1381,25 +1414,25 @@
       <c r="A30" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="12">
         <v>82</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="12">
         <v>84</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="12">
         <v>84.4</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="12">
         <v>84</v>
       </c>
-      <c r="F30" s="11">
-        <v>86</v>
-      </c>
-      <c r="G30" s="12">
-        <v>86</v>
-      </c>
-      <c r="H30">
+      <c r="F30" s="13">
+        <v>86</v>
+      </c>
+      <c r="G30" s="14">
+        <v>86</v>
+      </c>
+      <c r="H30" s="3">
         <v>86</v>
       </c>
     </row>
@@ -1407,25 +1440,25 @@
       <c r="A31" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="10">
-        <v>86</v>
-      </c>
-      <c r="C31" s="10">
-        <v>88</v>
-      </c>
-      <c r="D31" s="10">
+      <c r="B31" s="12">
+        <v>86</v>
+      </c>
+      <c r="C31" s="12">
+        <v>88</v>
+      </c>
+      <c r="D31" s="12">
         <v>88.5</v>
       </c>
-      <c r="E31" s="10">
-        <v>88</v>
-      </c>
-      <c r="F31" s="11">
+      <c r="E31" s="12">
+        <v>88</v>
+      </c>
+      <c r="F31" s="13">
         <v>88.9</v>
       </c>
-      <c r="G31" s="12">
+      <c r="G31" s="14">
         <v>89</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="3">
         <v>89</v>
       </c>
     </row>
@@ -1433,25 +1466,25 @@
       <c r="A32" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="12">
         <v>62</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="12">
         <v>63</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="12">
         <v>70.7</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="12">
         <v>63</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="13">
         <v>71.3</v>
       </c>
-      <c r="G32" s="12">
+      <c r="G32" s="14">
         <v>74</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="3">
         <v>81</v>
       </c>
     </row>
@@ -1459,25 +1492,25 @@
       <c r="A33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="10">
-        <v>86</v>
-      </c>
-      <c r="C33" s="10">
-        <v>86</v>
-      </c>
-      <c r="D33" s="10">
+      <c r="B33" s="12">
+        <v>86</v>
+      </c>
+      <c r="C33" s="12">
+        <v>86</v>
+      </c>
+      <c r="D33" s="12">
         <v>87.3</v>
       </c>
-      <c r="E33" s="10">
-        <v>86</v>
-      </c>
-      <c r="F33" s="11">
+      <c r="E33" s="12">
+        <v>86</v>
+      </c>
+      <c r="F33" s="13">
         <v>88.1</v>
       </c>
-      <c r="G33" s="12">
-        <v>88</v>
-      </c>
-      <c r="H33">
+      <c r="G33" s="14">
+        <v>88</v>
+      </c>
+      <c r="H33" s="3">
         <v>89</v>
       </c>
     </row>
@@ -1485,25 +1518,25 @@
       <c r="A34" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="12">
         <v>83</v>
       </c>
-      <c r="C34" s="10">
-        <v>86</v>
-      </c>
-      <c r="D34" s="10">
+      <c r="C34" s="12">
+        <v>86</v>
+      </c>
+      <c r="D34" s="12">
         <v>87.5</v>
       </c>
-      <c r="E34" s="10">
-        <v>86</v>
-      </c>
-      <c r="F34" s="11">
+      <c r="E34" s="12">
+        <v>86</v>
+      </c>
+      <c r="F34" s="13">
         <v>89.7</v>
       </c>
-      <c r="G34" s="12">
+      <c r="G34" s="14">
         <v>90</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="3">
         <v>91</v>
       </c>
     </row>
@@ -1511,25 +1544,25 @@
       <c r="A35" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="12">
         <v>63</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="12">
         <v>70</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="12">
         <v>70.3</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="12">
         <v>70</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F35" s="13">
         <v>68.599999999999994</v>
       </c>
-      <c r="G35" s="12">
+      <c r="G35" s="14">
         <v>71</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="3">
         <v>71</v>
       </c>
     </row>
@@ -1537,25 +1570,25 @@
       <c r="A36" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="12">
         <v>77</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="12">
         <v>77</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="12">
         <v>76.8</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="12">
         <v>77</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="13">
         <v>79.2</v>
       </c>
-      <c r="G36" s="12">
+      <c r="G36" s="14">
         <v>80</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="3">
         <v>82</v>
       </c>
     </row>
@@ -1563,25 +1596,25 @@
       <c r="A37" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="12">
         <v>78</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="12">
         <v>80</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D37" s="12">
         <v>82.5</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37" s="12">
         <v>80</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F37" s="13">
         <v>85.6</v>
       </c>
-      <c r="G37" s="12">
-        <v>86</v>
-      </c>
-      <c r="H37">
+      <c r="G37" s="14">
+        <v>86</v>
+      </c>
+      <c r="H37" s="3">
         <v>87</v>
       </c>
     </row>
@@ -1589,25 +1622,25 @@
       <c r="A38" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="10">
-        <v>86</v>
-      </c>
-      <c r="C38" s="10">
-        <v>87</v>
-      </c>
-      <c r="D38" s="10">
+      <c r="B38" s="12">
+        <v>86</v>
+      </c>
+      <c r="C38" s="12">
+        <v>87</v>
+      </c>
+      <c r="D38" s="12">
         <v>87.5</v>
       </c>
-      <c r="E38" s="10">
-        <v>87</v>
-      </c>
-      <c r="F38" s="11">
+      <c r="E38" s="12">
+        <v>87</v>
+      </c>
+      <c r="F38" s="13">
         <v>86.6</v>
       </c>
-      <c r="G38" s="12">
-        <v>88</v>
-      </c>
-      <c r="H38">
+      <c r="G38" s="14">
+        <v>88</v>
+      </c>
+      <c r="H38" s="3">
         <v>87</v>
       </c>
     </row>
@@ -1615,25 +1648,25 @@
       <c r="A39" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B39" s="12">
         <v>80</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="12">
         <v>81</v>
       </c>
-      <c r="D39" s="10">
+      <c r="D39" s="12">
         <v>82.2</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E39" s="12">
         <v>81</v>
       </c>
-      <c r="F39" s="11">
+      <c r="F39" s="13">
         <v>80.7</v>
       </c>
-      <c r="G39" s="12">
+      <c r="G39" s="14">
         <v>84</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="3">
         <v>84</v>
       </c>
     </row>
@@ -1641,19 +1674,25 @@
       <c r="A40" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="10">
+      <c r="B40" s="15">
+        <v>83.07</v>
+      </c>
+      <c r="C40" s="15">
+        <v>83.07</v>
+      </c>
+      <c r="D40" s="12">
         <v>84.8</v>
       </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="11">
+      <c r="E40" s="15">
+        <v>83.07</v>
+      </c>
+      <c r="F40" s="13">
         <v>82.5</v>
       </c>
-      <c r="G40" s="12">
+      <c r="G40" s="14">
         <v>82</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="3">
         <v>83</v>
       </c>
     </row>
@@ -1661,25 +1700,25 @@
       <c r="A41" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B41" s="12">
         <v>68</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="12">
         <v>68</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D41" s="12">
         <v>68.7</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E41" s="12">
         <v>68</v>
       </c>
-      <c r="F41" s="11">
+      <c r="F41" s="13">
         <v>73.8</v>
       </c>
-      <c r="G41" s="12">
+      <c r="G41" s="14">
         <v>75</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="3">
         <v>77</v>
       </c>
     </row>
@@ -1687,25 +1726,25 @@
       <c r="A42" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="12">
         <v>83</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="12">
         <v>84</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="12">
         <v>85.5</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42" s="12">
         <v>84</v>
       </c>
-      <c r="F42" s="11">
+      <c r="F42" s="13">
         <v>84.8</v>
       </c>
-      <c r="G42" s="12">
-        <v>86</v>
-      </c>
-      <c r="H42">
+      <c r="G42" s="14">
+        <v>86</v>
+      </c>
+      <c r="H42" s="3">
         <v>87</v>
       </c>
     </row>
@@ -1713,25 +1752,25 @@
       <c r="A43" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="12">
         <v>77</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="12">
         <v>77</v>
       </c>
-      <c r="D43" s="10">
+      <c r="D43" s="12">
         <v>79.7</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43" s="12">
         <v>77</v>
       </c>
-      <c r="F43" s="11">
+      <c r="F43" s="13">
         <v>83.2</v>
       </c>
-      <c r="G43" s="12">
+      <c r="G43" s="14">
         <v>83</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="3">
         <v>84</v>
       </c>
     </row>
@@ -1739,25 +1778,25 @@
       <c r="A44" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="12">
         <v>74</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="12">
         <v>75</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="12">
         <v>77.599999999999994</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="12">
         <v>75</v>
       </c>
-      <c r="F44" s="11">
+      <c r="F44" s="13">
         <v>80.3</v>
       </c>
-      <c r="G44" s="12">
+      <c r="G44" s="14">
         <v>83</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="3">
         <v>84</v>
       </c>
     </row>
@@ -1765,25 +1804,25 @@
       <c r="A45" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="12">
         <v>83</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="12">
         <v>83</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D45" s="12">
         <v>82.7</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="12">
         <v>83</v>
       </c>
-      <c r="F45" s="11">
+      <c r="F45" s="13">
         <v>83.9</v>
       </c>
-      <c r="G45" s="12">
+      <c r="G45" s="14">
         <v>84</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="3">
         <v>84</v>
       </c>
     </row>
@@ -1791,25 +1830,25 @@
       <c r="A46" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="10">
-        <v>86</v>
-      </c>
-      <c r="C46" s="10">
-        <v>87</v>
-      </c>
-      <c r="D46" s="10">
+      <c r="B46" s="12">
+        <v>86</v>
+      </c>
+      <c r="C46" s="12">
+        <v>87</v>
+      </c>
+      <c r="D46" s="12">
         <v>86.3</v>
       </c>
-      <c r="E46" s="10">
-        <v>87</v>
-      </c>
-      <c r="F46" s="11">
+      <c r="E46" s="12">
+        <v>87</v>
+      </c>
+      <c r="F46" s="13">
         <v>87.9</v>
       </c>
-      <c r="G46" s="12">
+      <c r="G46" s="14">
         <v>89</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="3">
         <v>90</v>
       </c>
     </row>
@@ -1817,25 +1856,25 @@
       <c r="A47" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="10">
-        <v>86</v>
-      </c>
-      <c r="C47" s="10">
-        <v>88</v>
-      </c>
-      <c r="D47" s="10">
-        <v>88</v>
-      </c>
-      <c r="E47" s="10">
-        <v>88</v>
-      </c>
-      <c r="F47" s="11">
+      <c r="B47" s="12">
+        <v>86</v>
+      </c>
+      <c r="C47" s="12">
+        <v>88</v>
+      </c>
+      <c r="D47" s="12">
+        <v>88</v>
+      </c>
+      <c r="E47" s="12">
+        <v>88</v>
+      </c>
+      <c r="F47" s="13">
         <v>89</v>
       </c>
-      <c r="G47" s="12">
+      <c r="G47" s="14">
         <v>89</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="3">
         <v>90</v>
       </c>
     </row>
@@ -1843,25 +1882,25 @@
       <c r="A48" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="10">
+      <c r="B48" s="12">
         <v>76</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C48" s="12">
         <v>80</v>
       </c>
-      <c r="D48" s="10">
+      <c r="D48" s="12">
         <v>83</v>
       </c>
-      <c r="E48" s="10">
+      <c r="E48" s="12">
         <v>80</v>
       </c>
-      <c r="F48" s="11">
+      <c r="F48" s="13">
         <v>84.8</v>
       </c>
-      <c r="G48" s="12">
+      <c r="G48" s="14">
         <v>85</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="3">
         <v>86</v>
       </c>
     </row>
@@ -1869,25 +1908,25 @@
       <c r="A49" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="10">
-        <v>87</v>
-      </c>
-      <c r="C49" s="10">
-        <v>88</v>
-      </c>
-      <c r="D49" s="10">
+      <c r="B49" s="12">
+        <v>87</v>
+      </c>
+      <c r="C49" s="12">
+        <v>88</v>
+      </c>
+      <c r="D49" s="12">
         <v>86.6</v>
       </c>
-      <c r="E49" s="10">
-        <v>88</v>
-      </c>
-      <c r="F49" s="11">
+      <c r="E49" s="12">
+        <v>88</v>
+      </c>
+      <c r="F49" s="13">
         <v>87.7</v>
       </c>
-      <c r="G49" s="12">
-        <v>88</v>
-      </c>
-      <c r="H49">
+      <c r="G49" s="14">
+        <v>88</v>
+      </c>
+      <c r="H49" s="3">
         <v>89</v>
       </c>
     </row>
@@ -1895,25 +1934,25 @@
       <c r="A50" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="10">
+      <c r="B50" s="12">
         <v>82</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C50" s="12">
         <v>83</v>
       </c>
-      <c r="D50" s="10">
+      <c r="D50" s="12">
         <v>84.5</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E50" s="12">
         <v>83</v>
       </c>
-      <c r="F50" s="11">
+      <c r="F50" s="13">
         <v>85.7</v>
       </c>
-      <c r="G50" s="12">
-        <v>87</v>
-      </c>
-      <c r="H50">
+      <c r="G50" s="14">
+        <v>87</v>
+      </c>
+      <c r="H50" s="3">
         <v>87</v>
       </c>
     </row>
@@ -1921,25 +1960,25 @@
       <c r="A51" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="10">
+      <c r="B51" s="12">
         <v>76</v>
       </c>
-      <c r="C51" s="10">
+      <c r="C51" s="12">
         <v>77</v>
       </c>
-      <c r="D51" s="10">
+      <c r="D51" s="12">
         <v>76.400000000000006</v>
       </c>
-      <c r="E51" s="10">
+      <c r="E51" s="12">
         <v>77</v>
       </c>
-      <c r="F51" s="11">
+      <c r="F51" s="13">
         <v>78.2</v>
       </c>
-      <c r="G51" s="12">
+      <c r="G51" s="14">
         <v>80</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="3">
         <v>79</v>
       </c>
     </row>
@@ -1947,25 +1986,25 @@
       <c r="A52" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B52" s="10">
+      <c r="B52" s="12">
         <v>78</v>
       </c>
-      <c r="C52" s="10">
+      <c r="C52" s="12">
         <v>79</v>
       </c>
-      <c r="D52" s="10">
+      <c r="D52" s="12">
         <v>81.400000000000006</v>
       </c>
-      <c r="E52" s="10">
+      <c r="E52" s="12">
         <v>79</v>
       </c>
-      <c r="F52" s="11">
+      <c r="F52" s="13">
         <v>86.5</v>
       </c>
-      <c r="G52" s="12">
+      <c r="G52" s="14">
         <v>90</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="3">
         <v>89</v>
       </c>
     </row>
@@ -1973,25 +2012,25 @@
       <c r="A53" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B53" s="10">
-        <v>87</v>
-      </c>
-      <c r="C53" s="10">
-        <v>88</v>
-      </c>
-      <c r="D53" s="10">
-        <v>88</v>
-      </c>
-      <c r="E53" s="10">
-        <v>88</v>
-      </c>
-      <c r="F53" s="11">
+      <c r="B53" s="12">
+        <v>87</v>
+      </c>
+      <c r="C53" s="12">
+        <v>88</v>
+      </c>
+      <c r="D53" s="12">
+        <v>88</v>
+      </c>
+      <c r="E53" s="12">
+        <v>88</v>
+      </c>
+      <c r="F53" s="13">
         <v>88.4</v>
       </c>
-      <c r="G53" s="12">
-        <v>88</v>
-      </c>
-      <c r="H53">
+      <c r="G53" s="14">
+        <v>88</v>
+      </c>
+      <c r="H53" s="3">
         <v>89</v>
       </c>
     </row>
@@ -1999,25 +2038,25 @@
       <c r="A54" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="14">
+      <c r="B54" s="16">
         <v>80</v>
       </c>
-      <c r="C54" s="14">
+      <c r="C54" s="16">
         <v>79</v>
       </c>
-      <c r="D54" s="14">
+      <c r="D54" s="16">
         <v>77</v>
       </c>
-      <c r="E54" s="14">
+      <c r="E54" s="16">
         <v>79</v>
       </c>
-      <c r="F54" s="15">
+      <c r="F54" s="17">
         <v>79.3</v>
       </c>
-      <c r="G54" s="12">
+      <c r="G54" s="14">
         <v>80</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="3">
         <v>86</v>
       </c>
     </row>

</xml_diff>